<commit_message>
Doing what mosi wants
</commit_message>
<xml_diff>
--- a/bullets.xlsx
+++ b/bullets.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,10 +430,6 @@
       <c r="B1" t="inlineStr"/>
       <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,18 +452,6 @@
           <t>Fast-paced</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Younger</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Working with a team</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -477,31 +461,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Leading projects</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>I care about and understand the work I am doing</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Calculate pricing and profit-maximizing</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Being a liaison between customer and technical resources</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Customer facing</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t>this is a very very very long question that cannot be answered easily by any person living on earth</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -509,41 +473,9 @@
           <t>what am I doing or what is happening around me?</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>When I am the happiest at work</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>The team I’m around is accomplishing goals</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Growth in my business</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>happy hours</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>dinners</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Growing relationships</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -553,23 +485,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Identifying customer needs</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Breaking glass in case of emergency to solve a customer problem</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Helping people on my team that are stuck</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -577,29 +497,9 @@
           <t>processes or things do I want to be responsible for?</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>What kind of people</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Generating leads</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>I like to work with inexperienced coworkers to help get them up to speed</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Short-term projects</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -607,25 +507,9 @@
           <t>What are the skills or knowledge or expertise I like to use the most?</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Being in the office and being around other people</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Salary</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Time-off</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>